<commit_message>
Cap nhat bang ke hoach
</commit_message>
<xml_diff>
--- a/BangKeHoach-DoAn1.xlsx
+++ b/BangKeHoach-DoAn1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\N3\Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD18CC6-81BA-4367-B8A9-13964FD97919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Kế Hoạch" sheetId="1" r:id="rId1"/>
@@ -184,7 +183,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
@@ -286,11 +285,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,7 +321,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Kế Hoạch-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Kế Hoạch-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -635,11 +634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -650,22 +649,22 @@
     <col min="4" max="4" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="23" width="8.6640625" style="2" customWidth="1"/>
     <col min="24" max="16384" width="14.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22.8" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -683,16 +682,16 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="22.8" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -845,8 +844,12 @@
       <c r="F6" s="7">
         <v>43749</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="7">
+        <v>43748</v>
+      </c>
+      <c r="H6" s="7">
+        <v>43779</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1365,10 +1368,10 @@
       <c r="D22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <v>43764</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <v>43764</v>
       </c>
       <c r="G22" s="7"/>

</xml_diff>